<commit_message>
Modified appendix table to include Wolfe et al. 2023 silver carp
</commit_message>
<xml_diff>
--- a/data/Appendix_ThiaminaseManuscript.xlsx
+++ b/data/Appendix_ThiaminaseManuscript.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/frowland_usgs_gov/Documents/Documents/Thiamine/Thiaminase manuscript/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/frowland_usgs_gov/Documents/Documents/Repositories/Thiaminase/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{113F9BC9-2768-4502-8290-5D6AF5AA9653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8EBFF92-A263-4B86-9EF2-B1C161B0B780}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{113F9BC9-2768-4502-8290-5D6AF5AA9653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEADEB75-4037-47EA-9332-4B79558C28BE}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="915" windowWidth="29040" windowHeight="15840" xr2:uid="{34A8F79B-2266-48D6-B1E4-BEF238EB0208}"/>
+    <workbookView xWindow="9450" yWindow="0" windowWidth="19110" windowHeight="15600" xr2:uid="{34A8F79B-2266-48D6-B1E4-BEF238EB0208}"/>
   </bookViews>
   <sheets>
     <sheet name="AllData" sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3528" uniqueCount="890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3538" uniqueCount="893">
   <si>
     <t>Common</t>
   </si>
@@ -2837,12 +2837,21 @@
   <si>
     <t>Median omega-3 (g/100 g) listed in fishbase.de</t>
   </si>
+  <si>
+    <t>Silver Carp</t>
+  </si>
+  <si>
+    <t>Hypophthalmichthys molitrix</t>
+  </si>
+  <si>
+    <t>Wolfe et al. 2023</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2877,12 +2886,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <i/>
@@ -3299,10 +3302,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F9AF0E-5470-4DF7-A3B0-BF75E05D72C4}">
-  <dimension ref="A1:W303"/>
+  <dimension ref="A1:W304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AM304" sqref="AM304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25746,9 +25750,81 @@
         <v>0.8</v>
       </c>
     </row>
+    <row r="304" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A304" s="6" t="s">
+        <v>890</v>
+      </c>
+      <c r="B304" s="6" t="s">
+        <v>891</v>
+      </c>
+      <c r="C304" s="6" t="s">
+        <v>892</v>
+      </c>
+      <c r="D304" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E304" t="s">
+        <v>27</v>
+      </c>
+      <c r="F304" t="s">
+        <v>28</v>
+      </c>
+      <c r="G304">
+        <v>0</v>
+      </c>
+      <c r="H304" t="s">
+        <v>50</v>
+      </c>
+      <c r="I304" t="s">
+        <v>45</v>
+      </c>
+      <c r="J304">
+        <v>1</v>
+      </c>
+      <c r="K304">
+        <v>0</v>
+      </c>
+      <c r="L304">
+        <v>1</v>
+      </c>
+      <c r="M304">
+        <v>0</v>
+      </c>
+      <c r="N304" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O304">
+        <v>0</v>
+      </c>
+      <c r="P304">
+        <v>1</v>
+      </c>
+      <c r="Q304">
+        <v>0</v>
+      </c>
+      <c r="R304">
+        <v>1</v>
+      </c>
+      <c r="S304" t="s">
+        <v>33</v>
+      </c>
+      <c r="T304">
+        <v>2</v>
+      </c>
+      <c r="U304">
+        <v>120</v>
+      </c>
+      <c r="V304">
+        <v>20</v>
+      </c>
+      <c r="W304">
+        <v>0.30599999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Minor changes to species info
</commit_message>
<xml_diff>
--- a/data/Appendix_ThiaminaseManuscript.xlsx
+++ b/data/Appendix_ThiaminaseManuscript.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="36" documentId="8_{113F9BC9-2768-4502-8290-5D6AF5AA9653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEADEB75-4037-47EA-9332-4B79558C28BE}"/>
   <bookViews>
-    <workbookView xWindow="9450" yWindow="0" windowWidth="19110" windowHeight="15600" xr2:uid="{34A8F79B-2266-48D6-B1E4-BEF238EB0208}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{34A8F79B-2266-48D6-B1E4-BEF238EB0208}"/>
   </bookViews>
   <sheets>
     <sheet name="AllData" sheetId="1" r:id="rId1"/>
@@ -2959,9 +2959,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2999,7 +2999,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3105,7 +3105,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3247,7 +3247,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3305,36 +3305,36 @@
   <dimension ref="A1:W304"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AM304" sqref="AM304"/>
+      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C203" sqref="C203"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="27" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="28.578125" style="6" customWidth="1"/>
     <col min="3" max="3" width="56" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.68359375" customWidth="1"/>
+    <col min="5" max="5" width="19.578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.15625" customWidth="1"/>
+    <col min="9" max="9" width="15.26171875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.41796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.26171875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.15625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="7.41796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.68359375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.26171875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.26171875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.26171875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.15625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.68359375" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="8.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
         <v>34</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
         <v>40</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6" t="s">
         <v>46</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>0.747</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6" t="s">
         <v>51</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>0.80800000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6" t="s">
         <v>55</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>9.2700000000000005E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="6" t="s">
         <v>59</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6" t="s">
         <v>65</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6" t="s">
         <v>69</v>
       </c>
@@ -4071,7 +4071,7 @@
         <v>2.67</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6" t="s">
         <v>72</v>
       </c>
@@ -4145,7 +4145,7 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6" t="s">
         <v>75</v>
       </c>
@@ -4219,7 +4219,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="6" t="s">
         <v>81</v>
       </c>
@@ -4293,7 +4293,7 @@
         <v>0.92700000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="6" t="s">
         <v>87</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>0.747</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6" t="s">
         <v>92</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="6" t="s">
         <v>95</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="6" t="s">
         <v>100</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>0.17299999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6" t="s">
         <v>102</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="6" t="s">
         <v>105</v>
       </c>
@@ -4737,7 +4737,7 @@
         <v>0.38800000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="6" t="s">
         <v>109</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>0.35199999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="6" t="s">
         <v>113</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="6" t="s">
         <v>115</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="6" t="s">
         <v>119</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="6" t="s">
         <v>123</v>
       </c>
@@ -5107,7 +5107,7 @@
         <v>0.75700000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="6" t="s">
         <v>125</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>0.77700000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="6" t="s">
         <v>31</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="6" t="s">
         <v>132</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="6" t="s">
         <v>135</v>
       </c>
@@ -5403,7 +5403,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="6" t="s">
         <v>140</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="6" t="s">
         <v>142</v>
       </c>
@@ -5551,7 +5551,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="6" t="s">
         <v>144</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="6" t="s">
         <v>31</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="6" t="s">
         <v>151</v>
       </c>
@@ -5773,7 +5773,7 @@
         <v>0.35799999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="6" t="s">
         <v>155</v>
       </c>
@@ -5847,7 +5847,7 @@
         <v>0.17100000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="6" t="s">
         <v>158</v>
       </c>
@@ -5921,7 +5921,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="6" t="s">
         <v>161</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="6" t="s">
         <v>164</v>
       </c>
@@ -6069,7 +6069,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="6" t="s">
         <v>167</v>
       </c>
@@ -6143,7 +6143,7 @@
         <v>0.55200000000000005</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="6" t="s">
         <v>169</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="6" t="s">
         <v>171</v>
       </c>
@@ -6291,7 +6291,7 @@
         <v>0.371</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="6" t="s">
         <v>175</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>0.48899999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="6" t="s">
         <v>180</v>
       </c>
@@ -6439,7 +6439,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="6" t="s">
         <v>183</v>
       </c>
@@ -6513,7 +6513,7 @@
         <v>0.29099999999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="6" t="s">
         <v>187</v>
       </c>
@@ -6587,7 +6587,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="6" t="s">
         <v>190</v>
       </c>
@@ -6661,7 +6661,7 @@
         <v>1.45</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="6" t="s">
         <v>193</v>
       </c>
@@ -6735,7 +6735,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="6" t="s">
         <v>198</v>
       </c>
@@ -6809,7 +6809,7 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="6" t="s">
         <v>202</v>
       </c>
@@ -6883,7 +6883,7 @@
         <v>0.35399999999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="6" t="s">
         <v>205</v>
       </c>
@@ -6957,7 +6957,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="6" t="s">
         <v>208</v>
       </c>
@@ -7031,7 +7031,7 @@
         <v>0.248</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="6" t="s">
         <v>212</v>
       </c>
@@ -7105,7 +7105,7 @@
         <v>7.7399999999999997E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="6" t="s">
         <v>215</v>
       </c>
@@ -7179,7 +7179,7 @@
         <v>0.318</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="6" t="s">
         <v>219</v>
       </c>
@@ -7253,7 +7253,7 @@
         <v>0.106</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="6" t="s">
         <v>223</v>
       </c>
@@ -7327,7 +7327,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="6" t="s">
         <v>226</v>
       </c>
@@ -7401,7 +7401,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="6" t="s">
         <v>229</v>
       </c>
@@ -7475,7 +7475,7 @@
         <v>0.746</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="6" t="s">
         <v>232</v>
       </c>
@@ -7549,7 +7549,7 @@
         <v>0.41299999999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="6" t="s">
         <v>234</v>
       </c>
@@ -7623,7 +7623,7 @@
         <v>0.20399999999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="6" t="s">
         <v>237</v>
       </c>
@@ -7697,7 +7697,7 @@
         <v>0.52300000000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="6" t="s">
         <v>240</v>
       </c>
@@ -7771,7 +7771,7 @@
         <v>0.46200000000000002</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="6" t="s">
         <v>243</v>
       </c>
@@ -7845,7 +7845,7 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="6" t="s">
         <v>248</v>
       </c>
@@ -7919,7 +7919,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="6" t="s">
         <v>250</v>
       </c>
@@ -7993,7 +7993,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="6" t="s">
         <v>252</v>
       </c>
@@ -8067,7 +8067,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="6" t="s">
         <v>255</v>
       </c>
@@ -8141,7 +8141,7 @@
         <v>0.22800000000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="6" t="s">
         <v>259</v>
       </c>
@@ -8215,7 +8215,7 @@
         <v>0.39900000000000002</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="6" t="s">
         <v>262</v>
       </c>
@@ -8289,7 +8289,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="6" t="s">
         <v>266</v>
       </c>
@@ -8363,7 +8363,7 @@
         <v>0.40799999999999997</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="6" t="s">
         <v>271</v>
       </c>
@@ -8437,7 +8437,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="6" t="s">
         <v>275</v>
       </c>
@@ -8511,7 +8511,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="6" t="s">
         <v>277</v>
       </c>
@@ -8585,7 +8585,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="6" t="s">
         <v>280</v>
       </c>
@@ -8659,7 +8659,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="6" t="s">
         <v>283</v>
       </c>
@@ -8733,7 +8733,7 @@
         <v>0.73099999999999998</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="6" t="s">
         <v>285</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>0.70899999999999996</v>
       </c>
     </row>
-    <row r="75" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="6" t="s">
         <v>288</v>
       </c>
@@ -8881,7 +8881,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="6" t="s">
         <v>291</v>
       </c>
@@ -8955,7 +8955,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="77" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="6" t="s">
         <v>294</v>
       </c>
@@ -9029,7 +9029,7 @@
         <v>0.33900000000000002</v>
       </c>
     </row>
-    <row r="78" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="6" t="s">
         <v>298</v>
       </c>
@@ -9103,7 +9103,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="79" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="6" t="s">
         <v>301</v>
       </c>
@@ -9177,7 +9177,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="6" t="s">
         <v>304</v>
       </c>
@@ -9251,7 +9251,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="6" t="s">
         <v>31</v>
       </c>
@@ -9325,7 +9325,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="6" t="s">
         <v>310</v>
       </c>
@@ -9399,7 +9399,7 @@
         <v>0.98899999999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="6" t="s">
         <v>312</v>
       </c>
@@ -9473,7 +9473,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="6" t="s">
         <v>314</v>
       </c>
@@ -9547,7 +9547,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="6" t="s">
         <v>316</v>
       </c>
@@ -9621,7 +9621,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="6" t="s">
         <v>321</v>
       </c>
@@ -9695,7 +9695,7 @@
         <v>0.63200000000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="6" t="s">
         <v>325</v>
       </c>
@@ -9769,7 +9769,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="6" t="s">
         <v>328</v>
       </c>
@@ -9843,7 +9843,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="6" t="s">
         <v>330</v>
       </c>
@@ -9917,7 +9917,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="6" t="s">
         <v>332</v>
       </c>
@@ -9991,7 +9991,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="6" t="s">
         <v>334</v>
       </c>
@@ -10065,7 +10065,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="6" t="s">
         <v>336</v>
       </c>
@@ -10139,7 +10139,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="6" t="s">
         <v>338</v>
       </c>
@@ -10213,7 +10213,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="6" t="s">
         <v>340</v>
       </c>
@@ -10287,7 +10287,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="6" t="s">
         <v>342</v>
       </c>
@@ -10361,7 +10361,7 @@
         <v>0.21099999999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="6" t="s">
         <v>347</v>
       </c>
@@ -10435,7 +10435,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="6" t="s">
         <v>351</v>
       </c>
@@ -10509,7 +10509,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="6" t="s">
         <v>354</v>
       </c>
@@ -10583,7 +10583,7 @@
         <v>0.95299999999999996</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="6" t="s">
         <v>357</v>
       </c>
@@ -10657,7 +10657,7 @@
         <v>0.25900000000000001</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="6" t="s">
         <v>360</v>
       </c>
@@ -10731,7 +10731,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="6" t="s">
         <v>363</v>
       </c>
@@ -10805,7 +10805,7 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="6" t="s">
         <v>367</v>
       </c>
@@ -10879,7 +10879,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="6" t="s">
         <v>31</v>
       </c>
@@ -10953,7 +10953,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="6" t="s">
         <v>372</v>
       </c>
@@ -11027,7 +11027,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="6" t="s">
         <v>376</v>
       </c>
@@ -11101,7 +11101,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="6" t="s">
         <v>379</v>
       </c>
@@ -11175,7 +11175,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="6" t="s">
         <v>31</v>
       </c>
@@ -11249,7 +11249,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="6" t="s">
         <v>383</v>
       </c>
@@ -11323,7 +11323,7 @@
         <v>0.499</v>
       </c>
     </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="6" t="s">
         <v>385</v>
       </c>
@@ -11397,7 +11397,7 @@
         <v>0.23799999999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="6" t="s">
         <v>388</v>
       </c>
@@ -11471,7 +11471,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="6" t="s">
         <v>392</v>
       </c>
@@ -11545,7 +11545,7 @@
         <v>0.64500000000000002</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="6" t="s">
         <v>395</v>
       </c>
@@ -11619,7 +11619,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="6" t="s">
         <v>398</v>
       </c>
@@ -11693,7 +11693,7 @@
         <v>0.36599999999999999</v>
       </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="6" t="s">
         <v>400</v>
       </c>
@@ -11767,7 +11767,7 @@
         <v>0.32100000000000001</v>
       </c>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="6" t="s">
         <v>402</v>
       </c>
@@ -11841,7 +11841,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="6" t="s">
         <v>404</v>
       </c>
@@ -11915,7 +11915,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="6" t="s">
         <v>406</v>
       </c>
@@ -11986,7 +11986,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="6" t="s">
         <v>410</v>
       </c>
@@ -12060,7 +12060,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="6" t="s">
         <v>415</v>
       </c>
@@ -12134,7 +12134,7 @@
         <v>0.40300000000000002</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="6" t="s">
         <v>31</v>
       </c>
@@ -12208,7 +12208,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="6" t="s">
         <v>418</v>
       </c>
@@ -12282,7 +12282,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="6" t="s">
         <v>420</v>
       </c>
@@ -12356,7 +12356,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="6" t="s">
         <v>422</v>
       </c>
@@ -12430,7 +12430,7 @@
         <v>0.35099999999999998</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="6" t="s">
         <v>424</v>
       </c>
@@ -12504,7 +12504,7 @@
         <v>0.29499999999999998</v>
       </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="6" t="s">
         <v>426</v>
       </c>
@@ -12578,7 +12578,7 @@
         <v>0.996</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="6" t="s">
         <v>428</v>
       </c>
@@ -12652,7 +12652,7 @@
         <v>0.40699999999999997</v>
       </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="6" t="s">
         <v>432</v>
       </c>
@@ -12726,7 +12726,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="6" t="s">
         <v>437</v>
       </c>
@@ -12800,7 +12800,7 @@
         <v>0.68400000000000005</v>
       </c>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="6" t="s">
         <v>439</v>
       </c>
@@ -12874,7 +12874,7 @@
         <v>0.51800000000000002</v>
       </c>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="6" t="s">
         <v>443</v>
       </c>
@@ -12948,7 +12948,7 @@
         <v>0.53200000000000003</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="6" t="s">
         <v>445</v>
       </c>
@@ -13022,7 +13022,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="6" t="s">
         <v>448</v>
       </c>
@@ -13096,7 +13096,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="6" t="s">
         <v>450</v>
       </c>
@@ -13170,7 +13170,7 @@
         <v>0.372</v>
       </c>
     </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="6" t="s">
         <v>453</v>
       </c>
@@ -13244,7 +13244,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="6" t="s">
         <v>455</v>
       </c>
@@ -13318,7 +13318,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="6" t="s">
         <v>457</v>
       </c>
@@ -13392,7 +13392,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="6" t="s">
         <v>460</v>
       </c>
@@ -13466,7 +13466,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="6" t="s">
         <v>462</v>
       </c>
@@ -13540,7 +13540,7 @@
         <v>0.34300000000000003</v>
       </c>
     </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="6" t="s">
         <v>464</v>
       </c>
@@ -13614,7 +13614,7 @@
         <v>0.61099999999999999</v>
       </c>
     </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="6" t="s">
         <v>467</v>
       </c>
@@ -13688,7 +13688,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="6" t="s">
         <v>471</v>
       </c>
@@ -13762,7 +13762,7 @@
         <v>0.66600000000000004</v>
       </c>
     </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="6" t="s">
         <v>473</v>
       </c>
@@ -13836,7 +13836,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="6" t="s">
         <v>477</v>
       </c>
@@ -13910,7 +13910,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="6" t="s">
         <v>479</v>
       </c>
@@ -13984,7 +13984,7 @@
         <v>0.91100000000000003</v>
       </c>
     </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="6" t="s">
         <v>481</v>
       </c>
@@ -14058,7 +14058,7 @@
         <v>0.314</v>
       </c>
     </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="6" t="s">
         <v>485</v>
       </c>
@@ -14132,7 +14132,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="6" t="s">
         <v>487</v>
       </c>
@@ -14206,7 +14206,7 @@
         <v>0.433</v>
       </c>
     </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="6" t="s">
         <v>491</v>
       </c>
@@ -14280,7 +14280,7 @@
         <v>0.434</v>
       </c>
     </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="6" t="s">
         <v>493</v>
       </c>
@@ -14354,7 +14354,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="6" t="s">
         <v>495</v>
       </c>
@@ -14428,7 +14428,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="6" t="s">
         <v>499</v>
       </c>
@@ -14502,7 +14502,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="6" t="s">
         <v>502</v>
       </c>
@@ -14576,7 +14576,7 @@
         <v>0.67900000000000005</v>
       </c>
     </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="6" t="s">
         <v>504</v>
       </c>
@@ -14650,7 +14650,7 @@
         <v>0.27700000000000002</v>
       </c>
     </row>
-    <row r="154" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="6" t="s">
         <v>507</v>
       </c>
@@ -14724,7 +14724,7 @@
         <v>0.60699999999999998</v>
       </c>
     </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="6" t="s">
         <v>509</v>
       </c>
@@ -14798,7 +14798,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="156" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="6" t="s">
         <v>511</v>
       </c>
@@ -14872,7 +14872,7 @@
         <v>0.39700000000000002</v>
       </c>
     </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="6" t="s">
         <v>514</v>
       </c>
@@ -14946,7 +14946,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="6" t="s">
         <v>517</v>
       </c>
@@ -15020,7 +15020,7 @@
         <v>0.313</v>
       </c>
     </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="6" t="s">
         <v>520</v>
       </c>
@@ -15094,7 +15094,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="6" t="s">
         <v>524</v>
       </c>
@@ -15168,7 +15168,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="161" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="6" t="s">
         <v>526</v>
       </c>
@@ -15242,7 +15242,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="162" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="6" t="s">
         <v>528</v>
       </c>
@@ -15316,7 +15316,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="163" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="6" t="s">
         <v>530</v>
       </c>
@@ -15390,7 +15390,7 @@
         <v>0.76100000000000001</v>
       </c>
     </row>
-    <row r="164" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="6" t="s">
         <v>535</v>
       </c>
@@ -15464,7 +15464,7 @@
         <v>1.18</v>
       </c>
     </row>
-    <row r="165" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="6" t="s">
         <v>537</v>
       </c>
@@ -15538,7 +15538,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="166" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="6" t="s">
         <v>539</v>
       </c>
@@ -15612,7 +15612,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="167" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="6" t="s">
         <v>542</v>
       </c>
@@ -15686,7 +15686,7 @@
         <v>0.13600000000000001</v>
       </c>
     </row>
-    <row r="168" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="6" t="s">
         <v>546</v>
       </c>
@@ -15760,7 +15760,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="169" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="6" t="s">
         <v>548</v>
       </c>
@@ -15834,7 +15834,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="170" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="6" t="s">
         <v>551</v>
       </c>
@@ -15908,7 +15908,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="171" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="6" t="s">
         <v>553</v>
       </c>
@@ -15982,7 +15982,7 @@
         <v>0.58499999999999996</v>
       </c>
     </row>
-    <row r="172" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="6" t="s">
         <v>555</v>
       </c>
@@ -16056,7 +16056,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="173" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="6" t="s">
         <v>557</v>
       </c>
@@ -16130,7 +16130,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="174" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="6" t="s">
         <v>559</v>
       </c>
@@ -16204,7 +16204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="6" t="s">
         <v>31</v>
       </c>
@@ -16278,7 +16278,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="176" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="6" t="s">
         <v>562</v>
       </c>
@@ -16352,7 +16352,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="177" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="6" t="s">
         <v>564</v>
       </c>
@@ -16426,7 +16426,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="178" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="6" t="s">
         <v>31</v>
       </c>
@@ -16500,7 +16500,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="179" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="6" t="s">
         <v>567</v>
       </c>
@@ -16574,7 +16574,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="180" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="6" t="s">
         <v>569</v>
       </c>
@@ -16648,7 +16648,7 @@
         <v>0.71399999999999997</v>
       </c>
     </row>
-    <row r="181" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="6" t="s">
         <v>571</v>
       </c>
@@ -16722,7 +16722,7 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="182" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="6" t="s">
         <v>573</v>
       </c>
@@ -16796,7 +16796,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="183" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="6" t="s">
         <v>575</v>
       </c>
@@ -16870,7 +16870,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="184" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="6" t="s">
         <v>578</v>
       </c>
@@ -16944,7 +16944,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="185" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="6" t="s">
         <v>580</v>
       </c>
@@ -17018,7 +17018,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="186" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="6" t="s">
         <v>582</v>
       </c>
@@ -17092,7 +17092,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="187" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="6" t="s">
         <v>584</v>
       </c>
@@ -17166,7 +17166,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="188" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="6" t="s">
         <v>586</v>
       </c>
@@ -17240,7 +17240,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="189" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="6" t="s">
         <v>31</v>
       </c>
@@ -17314,7 +17314,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="190" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="6" t="s">
         <v>590</v>
       </c>
@@ -17388,7 +17388,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="191" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="6" t="s">
         <v>592</v>
       </c>
@@ -17462,7 +17462,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="192" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="6" t="s">
         <v>594</v>
       </c>
@@ -17536,7 +17536,7 @@
         <v>1.44</v>
       </c>
     </row>
-    <row r="193" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="6" t="s">
         <v>596</v>
       </c>
@@ -17610,7 +17610,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="194" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="6" t="s">
         <v>598</v>
       </c>
@@ -17684,7 +17684,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="195" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="6" t="s">
         <v>31</v>
       </c>
@@ -17758,7 +17758,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="196" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="6" t="s">
         <v>601</v>
       </c>
@@ -17832,7 +17832,7 @@
         <v>0.42799999999999999</v>
       </c>
     </row>
-    <row r="197" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="6" t="s">
         <v>603</v>
       </c>
@@ -17906,7 +17906,7 @@
         <v>0.40699999999999997</v>
       </c>
     </row>
-    <row r="198" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="6" t="s">
         <v>605</v>
       </c>
@@ -17980,7 +17980,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="199" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="6" t="s">
         <v>608</v>
       </c>
@@ -18054,7 +18054,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="200" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="6" t="s">
         <v>610</v>
       </c>
@@ -18128,7 +18128,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="201" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="6" t="s">
         <v>612</v>
       </c>
@@ -18202,7 +18202,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="202" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" s="6" t="s">
         <v>614</v>
       </c>
@@ -18276,7 +18276,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="203" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" s="6" t="s">
         <v>617</v>
       </c>
@@ -18350,7 +18350,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="204" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="6" t="s">
         <v>620</v>
       </c>
@@ -18424,7 +18424,7 @@
         <v>0.28399999999999997</v>
       </c>
     </row>
-    <row r="205" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" s="6" t="s">
         <v>623</v>
       </c>
@@ -18498,7 +18498,7 @@
         <v>0.58899999999999997</v>
       </c>
     </row>
-    <row r="206" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="6" t="s">
         <v>31</v>
       </c>
@@ -18572,7 +18572,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="207" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" s="6" t="s">
         <v>629</v>
       </c>
@@ -18646,7 +18646,7 @@
         <v>0.30499999999999999</v>
       </c>
     </row>
-    <row r="208" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" s="6" t="s">
         <v>632</v>
       </c>
@@ -18720,7 +18720,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="209" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="6" t="s">
         <v>635</v>
       </c>
@@ -18794,7 +18794,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="210" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" s="6" t="s">
         <v>637</v>
       </c>
@@ -18868,7 +18868,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="211" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" s="6" t="s">
         <v>639</v>
       </c>
@@ -18942,7 +18942,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="212" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" s="6" t="s">
         <v>641</v>
       </c>
@@ -19016,7 +19016,7 @@
         <v>0.95699999999999996</v>
       </c>
     </row>
-    <row r="213" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="6" t="s">
         <v>643</v>
       </c>
@@ -19090,7 +19090,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="214" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="6" t="s">
         <v>646</v>
       </c>
@@ -19164,7 +19164,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="215" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" s="6" t="s">
         <v>648</v>
       </c>
@@ -19238,7 +19238,7 @@
         <v>0.65700000000000003</v>
       </c>
     </row>
-    <row r="216" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="6" t="s">
         <v>651</v>
       </c>
@@ -19312,7 +19312,7 @@
         <v>0.14299999999999999</v>
       </c>
     </row>
-    <row r="217" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="6" t="s">
         <v>653</v>
       </c>
@@ -19386,7 +19386,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="218" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" s="6" t="s">
         <v>655</v>
       </c>
@@ -19460,7 +19460,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="219" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="6" t="s">
         <v>657</v>
       </c>
@@ -19534,7 +19534,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="220" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" s="6" t="s">
         <v>659</v>
       </c>
@@ -19608,7 +19608,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="221" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" s="6" t="s">
         <v>661</v>
       </c>
@@ -19682,7 +19682,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="222" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="6" t="s">
         <v>663</v>
       </c>
@@ -19756,7 +19756,7 @@
         <v>0.58399999999999996</v>
       </c>
     </row>
-    <row r="223" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" s="6" t="s">
         <v>665</v>
       </c>
@@ -19830,7 +19830,7 @@
         <v>0.28499999999999998</v>
       </c>
     </row>
-    <row r="224" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" s="6" t="s">
         <v>668</v>
       </c>
@@ -19904,7 +19904,7 @@
         <v>0.22700000000000001</v>
       </c>
     </row>
-    <row r="225" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" s="6" t="s">
         <v>670</v>
       </c>
@@ -19978,7 +19978,7 @@
         <v>0.39700000000000002</v>
       </c>
     </row>
-    <row r="226" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="6" t="s">
         <v>672</v>
       </c>
@@ -20052,7 +20052,7 @@
         <v>0.78100000000000003</v>
       </c>
     </row>
-    <row r="227" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" s="6" t="s">
         <v>675</v>
       </c>
@@ -20126,7 +20126,7 @@
         <v>0.38700000000000001</v>
       </c>
     </row>
-    <row r="228" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" s="6" t="s">
         <v>678</v>
       </c>
@@ -20200,7 +20200,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" s="6" t="s">
         <v>681</v>
       </c>
@@ -20274,7 +20274,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" s="6" t="s">
         <v>685</v>
       </c>
@@ -20348,7 +20348,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="231" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" s="6" t="s">
         <v>688</v>
       </c>
@@ -20422,7 +20422,7 @@
         <v>0.35899999999999999</v>
       </c>
     </row>
-    <row r="232" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" s="6" t="s">
         <v>688</v>
       </c>
@@ -20496,7 +20496,7 @@
         <v>0.35899999999999999</v>
       </c>
     </row>
-    <row r="233" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" s="6" t="s">
         <v>691</v>
       </c>
@@ -20570,7 +20570,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" s="6" t="s">
         <v>694</v>
       </c>
@@ -20644,7 +20644,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" s="6" t="s">
         <v>696</v>
       </c>
@@ -20718,7 +20718,7 @@
         <v>0.57199999999999995</v>
       </c>
     </row>
-    <row r="236" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" s="6" t="s">
         <v>698</v>
       </c>
@@ -20792,7 +20792,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" s="6" t="s">
         <v>701</v>
       </c>
@@ -20866,7 +20866,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="238" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="6" t="s">
         <v>703</v>
       </c>
@@ -20940,7 +20940,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="239" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" s="6" t="s">
         <v>31</v>
       </c>
@@ -21014,7 +21014,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="240" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="6" t="s">
         <v>707</v>
       </c>
@@ -21088,7 +21088,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="241" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="6" t="s">
         <v>709</v>
       </c>
@@ -21162,7 +21162,7 @@
         <v>0.186</v>
       </c>
     </row>
-    <row r="242" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" s="6" t="s">
         <v>713</v>
       </c>
@@ -21236,7 +21236,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="243" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="6" t="s">
         <v>715</v>
       </c>
@@ -21310,7 +21310,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="244" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" s="6" t="s">
         <v>717</v>
       </c>
@@ -21384,7 +21384,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="245" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="6" t="s">
         <v>719</v>
       </c>
@@ -21458,7 +21458,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="246" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" s="6" t="s">
         <v>721</v>
       </c>
@@ -21532,7 +21532,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="247" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" s="6" t="s">
         <v>723</v>
       </c>
@@ -21606,7 +21606,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="248" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A248" s="6" t="s">
         <v>725</v>
       </c>
@@ -21680,7 +21680,7 @@
         <v>0.42899999999999999</v>
       </c>
     </row>
-    <row r="249" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A249" s="6" t="s">
         <v>728</v>
       </c>
@@ -21754,7 +21754,7 @@
         <v>0.76500000000000001</v>
       </c>
     </row>
-    <row r="250" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A250" s="6" t="s">
         <v>730</v>
       </c>
@@ -21828,7 +21828,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="251" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A251" s="6" t="s">
         <v>732</v>
       </c>
@@ -21902,7 +21902,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="252" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A252" s="6" t="s">
         <v>735</v>
       </c>
@@ -21976,7 +21976,7 @@
         <v>0.39700000000000002</v>
       </c>
     </row>
-    <row r="253" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" s="6" t="s">
         <v>737</v>
       </c>
@@ -22050,7 +22050,7 @@
         <v>1.34</v>
       </c>
     </row>
-    <row r="254" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A254" s="6" t="s">
         <v>739</v>
       </c>
@@ -22124,7 +22124,7 @@
         <v>0.59199999999999997</v>
       </c>
     </row>
-    <row r="255" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" s="6" t="s">
         <v>742</v>
       </c>
@@ -22198,7 +22198,7 @@
         <v>0.20200000000000001</v>
       </c>
     </row>
-    <row r="256" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A256" s="6" t="s">
         <v>746</v>
       </c>
@@ -22272,7 +22272,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="257" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" s="6" t="s">
         <v>749</v>
       </c>
@@ -22346,7 +22346,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="258" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" s="6" t="s">
         <v>751</v>
       </c>
@@ -22420,7 +22420,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="259" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" s="6" t="s">
         <v>753</v>
       </c>
@@ -22494,7 +22494,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="260" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" s="6" t="s">
         <v>753</v>
       </c>
@@ -22568,7 +22568,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="261" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" s="6" t="s">
         <v>755</v>
       </c>
@@ -22642,7 +22642,7 @@
         <v>0.224</v>
       </c>
     </row>
-    <row r="262" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A262" s="6" t="s">
         <v>757</v>
       </c>
@@ -22716,7 +22716,7 @@
         <v>0.67900000000000005</v>
       </c>
     </row>
-    <row r="263" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" s="6" t="s">
         <v>759</v>
       </c>
@@ -22790,7 +22790,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="264" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A264" s="6" t="s">
         <v>762</v>
       </c>
@@ -22864,7 +22864,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="265" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A265" s="6" t="s">
         <v>31</v>
       </c>
@@ -22938,7 +22938,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="266" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" s="6" t="s">
         <v>765</v>
       </c>
@@ -23012,7 +23012,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="267" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A267" s="6" t="s">
         <v>31</v>
       </c>
@@ -23086,7 +23086,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="268" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A268" s="6" t="s">
         <v>769</v>
       </c>
@@ -23160,7 +23160,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="269" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A269" s="6" t="s">
         <v>31</v>
       </c>
@@ -23234,7 +23234,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="270" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A270" s="6" t="s">
         <v>772</v>
       </c>
@@ -23308,7 +23308,7 @@
         <v>0.158</v>
       </c>
     </row>
-    <row r="271" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A271" s="6" t="s">
         <v>775</v>
       </c>
@@ -23382,7 +23382,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="272" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A272" s="6" t="s">
         <v>777</v>
       </c>
@@ -23456,7 +23456,7 @@
         <v>0.16300000000000001</v>
       </c>
     </row>
-    <row r="273" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A273" s="6" t="s">
         <v>781</v>
       </c>
@@ -23530,7 +23530,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="274" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A274" s="6" t="s">
         <v>784</v>
       </c>
@@ -23604,7 +23604,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="275" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A275" s="6" t="s">
         <v>788</v>
       </c>
@@ -23678,7 +23678,7 @@
         <v>0.14099999999999999</v>
       </c>
     </row>
-    <row r="276" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A276" s="6" t="s">
         <v>790</v>
       </c>
@@ -23752,7 +23752,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="277" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A277" s="6" t="s">
         <v>792</v>
       </c>
@@ -23826,7 +23826,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="278" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A278" s="6" t="s">
         <v>795</v>
       </c>
@@ -23900,7 +23900,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="279" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A279" s="6" t="s">
         <v>799</v>
       </c>
@@ -23974,7 +23974,7 @@
         <v>0.55300000000000005</v>
       </c>
     </row>
-    <row r="280" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A280" s="6" t="s">
         <v>801</v>
       </c>
@@ -24048,7 +24048,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="281" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A281" s="6" t="s">
         <v>31</v>
       </c>
@@ -24122,7 +24122,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="282" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A282" s="6" t="s">
         <v>806</v>
       </c>
@@ -24196,7 +24196,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="283" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" s="6" t="s">
         <v>808</v>
       </c>
@@ -24270,7 +24270,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="284" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A284" s="6" t="s">
         <v>810</v>
       </c>
@@ -24344,7 +24344,7 @@
         <v>0.34200000000000003</v>
       </c>
     </row>
-    <row r="285" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" s="6" t="s">
         <v>812</v>
       </c>
@@ -24418,7 +24418,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="286" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A286" s="6" t="s">
         <v>814</v>
       </c>
@@ -24492,7 +24492,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="287" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A287" s="6" t="s">
         <v>31</v>
       </c>
@@ -24566,7 +24566,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="288" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" s="6" t="s">
         <v>819</v>
       </c>
@@ -24640,7 +24640,7 @@
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="289" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A289" s="6" t="s">
         <v>822</v>
       </c>
@@ -24714,7 +24714,7 @@
         <v>0.57299999999999995</v>
       </c>
     </row>
-    <row r="290" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A290" s="6" t="s">
         <v>824</v>
       </c>
@@ -24788,7 +24788,7 @@
         <v>0.63900000000000001</v>
       </c>
     </row>
-    <row r="291" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" s="6" t="s">
         <v>826</v>
       </c>
@@ -24862,7 +24862,7 @@
         <v>1.49</v>
       </c>
     </row>
-    <row r="292" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A292" s="6" t="s">
         <v>829</v>
       </c>
@@ -24936,7 +24936,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="293" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A293" s="6" t="s">
         <v>832</v>
       </c>
@@ -25010,7 +25010,7 @@
         <v>0.35899999999999999</v>
       </c>
     </row>
-    <row r="294" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A294" s="6" t="s">
         <v>834</v>
       </c>
@@ -25084,7 +25084,7 @@
         <v>0.44700000000000001</v>
       </c>
     </row>
-    <row r="295" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A295" s="6" t="s">
         <v>31</v>
       </c>
@@ -25158,7 +25158,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="296" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A296" s="6" t="s">
         <v>840</v>
       </c>
@@ -25232,7 +25232,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="297" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A297" s="6" t="s">
         <v>843</v>
       </c>
@@ -25306,7 +25306,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="298" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A298" s="6" t="s">
         <v>846</v>
       </c>
@@ -25380,7 +25380,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="299" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A299" s="6" t="s">
         <v>848</v>
       </c>
@@ -25454,7 +25454,7 @@
         <v>0.32200000000000001</v>
       </c>
     </row>
-    <row r="300" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A300" s="6" t="s">
         <v>851</v>
       </c>
@@ -25528,7 +25528,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="301" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A301" s="6" t="s">
         <v>853</v>
       </c>
@@ -25602,7 +25602,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="302" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A302" s="6" t="s">
         <v>855</v>
       </c>
@@ -25676,7 +25676,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="303" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A303" s="6" t="s">
         <v>857</v>
       </c>
@@ -25750,7 +25750,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="304" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A304" s="6" t="s">
         <v>890</v>
       </c>
@@ -25836,14 +25836,14 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="101.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83984375" customWidth="1"/>
+    <col min="3" max="3" width="101.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>860</v>
       </c>
@@ -25854,7 +25854,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -25865,7 +25865,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -25876,7 +25876,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -25887,7 +25887,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -25898,7 +25898,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -25909,7 +25909,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -25920,7 +25920,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -25931,7 +25931,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -25942,7 +25942,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -25953,7 +25953,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -25964,7 +25964,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -25975,7 +25975,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
@@ -25986,7 +25986,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -25997,7 +25997,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -26008,7 +26008,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -26019,7 +26019,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -26030,7 +26030,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -26041,7 +26041,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -26052,7 +26052,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -26063,7 +26063,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -26074,7 +26074,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -26085,7 +26085,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -26096,7 +26096,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>22</v>
       </c>

</xml_diff>